<commit_message>
create function convert general information
</commit_message>
<xml_diff>
--- a/client/src/data/assignment.xlsx
+++ b/client/src/data/assignment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nam4\KLTN\Project_ELearning_KLTN\server\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129C6E84-9474-49D4-B10B-A1D2FCD6E594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE97DA0-A234-450B-BC41-1C6D3AA15D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>title</t>
   </si>
@@ -131,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -141,6 +141,9 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -425,20 +428,20 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="21.21875" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,11 +461,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -478,13 +481,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
+    <row r="3" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
@@ -498,13 +497,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
+    <row r="4" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
@@ -518,11 +513,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -538,13 +533,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
+    <row r="6" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
@@ -558,13 +549,9 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
+    <row r="7" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
@@ -578,11 +565,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -598,13 +585,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>16</v>
-      </c>
+    <row r="9" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
@@ -618,13 +601,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>16</v>
-      </c>
+    <row r="10" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
@@ -638,7 +617,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -646,7 +625,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -654,7 +633,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -663,6 +642,14 @@
       <c r="F13" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>